<commit_message>
feat: sync updated code & template
</commit_message>
<xml_diff>
--- a/agenda_generator/ToastMaster_Template.xlsx
+++ b/agenda_generator/ToastMaster_Template.xlsx
@@ -1,29 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\STCVM-L31\share_folder\toastmaster_agenda_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D20765D-644D-452F-818E-829753D8CE76}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A947FBB3-E84E-43F7-9A3B-F77BA03AFD9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda-1" sheetId="7" r:id="rId1"/>
     <sheet name="Agenda-2" sheetId="10" r:id="rId2"/>
-    <sheet name="Chinese Agenda-1" sheetId="9" r:id="rId3"/>
-    <sheet name="Chinese Agenda-2" sheetId="8" r:id="rId4"/>
-    <sheet name="Roles" sheetId="5" r:id="rId5"/>
+    <sheet name="Agenda-3" sheetId="11" r:id="rId3"/>
+    <sheet name="Chinese Agenda-1" sheetId="9" r:id="rId4"/>
+    <sheet name="Chinese Agenda-2" sheetId="8" r:id="rId5"/>
+    <sheet name="Roles" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Agenda-1'!$A$1:$H$40</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Agenda-2'!$A$1:$H$43</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Chinese Agenda-1'!$A$1:$H$40</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Chinese Agenda-2'!$A$1:$H$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Agenda-3'!$A$1:$H$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Chinese Agenda-1'!$A$1:$H$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Chinese Agenda-2'!$A$1:$H$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="362">
   <si>
     <t>Welcome to Microsoft Beijing Toastmasters Club</t>
   </si>
@@ -1150,6 +1152,15 @@
   </si>
   <si>
     <t>语法官报告</t>
+  </si>
+  <si>
+    <t>Introduce the 3nd Speaker</t>
+  </si>
+  <si>
+    <t>Evaluate the 3rd speaker</t>
+  </si>
+  <si>
+    <t>Prepared Speaker3</t>
   </si>
 </sst>
 </file>
@@ -2843,7 +2854,7 @@
     <xf numFmtId="165" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="222">
+  <cellXfs count="229">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -3269,48 +3280,90 @@
     <xf numFmtId="167" fontId="8" fillId="0" borderId="7" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="48" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="17" fillId="0" borderId="7" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="46" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="19" fillId="3" borderId="7" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="8" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="8" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="46" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="3" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="17" fillId="0" borderId="5" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3365,25 +3418,11 @@
     <xf numFmtId="165" fontId="15" fillId="0" borderId="15" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="48" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="52" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="18" fontId="17" fillId="0" borderId="7" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="20" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="60" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="62" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="50" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3398,7 +3437,6 @@
     <xf numFmtId="167" fontId="50" fillId="0" borderId="5" xfId="20" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="60" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="61" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="61" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="61" fillId="0" borderId="0" xfId="20" applyFont="1"/>
@@ -3407,12 +3445,6 @@
     </xf>
     <xf numFmtId="167" fontId="50" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="52" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="62" fillId="0" borderId="0" xfId="20" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="349">
@@ -4153,108 +4185,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="198" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="181"/>
-      <c r="F1" s="182"/>
-      <c r="G1" s="183"/>
-      <c r="H1" s="184"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="190"/>
+      <c r="E1" s="193"/>
+      <c r="F1" s="194"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="196"/>
     </row>
     <row r="2" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A2" s="185" t="s">
+      <c r="A2" s="199" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="179"/>
-      <c r="C2" s="179"/>
-      <c r="D2" s="180"/>
-      <c r="E2" s="181"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="183"/>
-      <c r="H2" s="184"/>
+      <c r="B2" s="181"/>
+      <c r="C2" s="181"/>
+      <c r="D2" s="190"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="194"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="196"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A3" s="186" t="s">
+      <c r="A3" s="200" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="179"/>
-      <c r="C3" s="179"/>
-      <c r="D3" s="180"/>
-      <c r="E3" s="181"/>
-      <c r="F3" s="182"/>
-      <c r="G3" s="183"/>
-      <c r="H3" s="184"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="190"/>
+      <c r="E3" s="193"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="196"/>
       <c r="I3" s="35"/>
       <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A4" s="187" t="s">
+      <c r="A4" s="201" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="190" t="s">
+      <c r="B4" s="204" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="191"/>
-      <c r="D4" s="192"/>
-      <c r="E4" s="193"/>
-      <c r="F4" s="194"/>
-      <c r="G4" s="195"/>
-      <c r="H4" s="196"/>
+      <c r="C4" s="205"/>
+      <c r="D4" s="206"/>
+      <c r="E4" s="207"/>
+      <c r="F4" s="208"/>
+      <c r="G4" s="209"/>
+      <c r="H4" s="210"/>
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A5" s="188"/>
-      <c r="B5" s="191"/>
-      <c r="C5" s="191"/>
-      <c r="D5" s="192"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="195"/>
-      <c r="H5" s="196"/>
+      <c r="A5" s="202"/>
+      <c r="B5" s="205"/>
+      <c r="C5" s="205"/>
+      <c r="D5" s="206"/>
+      <c r="E5" s="207"/>
+      <c r="F5" s="208"/>
+      <c r="G5" s="209"/>
+      <c r="H5" s="210"/>
       <c r="I5" s="35"/>
       <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="22.5" hidden="1" customHeight="1">
-      <c r="A6" s="188"/>
-      <c r="B6" s="191"/>
-      <c r="C6" s="191"/>
-      <c r="D6" s="192"/>
-      <c r="E6" s="193"/>
-      <c r="F6" s="194"/>
-      <c r="G6" s="195"/>
-      <c r="H6" s="196"/>
+      <c r="A6" s="202"/>
+      <c r="B6" s="205"/>
+      <c r="C6" s="205"/>
+      <c r="D6" s="206"/>
+      <c r="E6" s="207"/>
+      <c r="F6" s="208"/>
+      <c r="G6" s="209"/>
+      <c r="H6" s="210"/>
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
     </row>
     <row r="7" spans="1:12" ht="10.5" hidden="1" customHeight="1">
-      <c r="A7" s="189"/>
-      <c r="B7" s="197"/>
-      <c r="C7" s="197"/>
-      <c r="D7" s="198"/>
-      <c r="E7" s="199"/>
-      <c r="F7" s="200"/>
-      <c r="G7" s="201"/>
-      <c r="H7" s="202"/>
+      <c r="A7" s="203"/>
+      <c r="B7" s="211"/>
+      <c r="C7" s="211"/>
+      <c r="D7" s="212"/>
+      <c r="E7" s="213"/>
+      <c r="F7" s="214"/>
+      <c r="G7" s="215"/>
+      <c r="H7" s="216"/>
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A8" s="171" t="s">
+      <c r="A8" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="172"/>
-      <c r="C8" s="172"/>
-      <c r="D8" s="173"/>
-      <c r="E8" s="174"/>
-      <c r="F8" s="175"/>
-      <c r="G8" s="176"/>
-      <c r="H8" s="177"/>
+      <c r="B8" s="183"/>
+      <c r="C8" s="183"/>
+      <c r="D8" s="184"/>
+      <c r="E8" s="185"/>
+      <c r="F8" s="186"/>
+      <c r="G8" s="187"/>
+      <c r="H8" s="188"/>
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
     </row>
@@ -4619,16 +4651,16 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A20" s="206" t="s">
+      <c r="A20" s="182" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="172"/>
-      <c r="C20" s="172"/>
-      <c r="D20" s="173"/>
-      <c r="E20" s="174"/>
-      <c r="F20" s="175"/>
-      <c r="G20" s="176"/>
-      <c r="H20" s="177"/>
+      <c r="B20" s="183"/>
+      <c r="C20" s="183"/>
+      <c r="D20" s="184"/>
+      <c r="E20" s="185"/>
+      <c r="F20" s="186"/>
+      <c r="G20" s="187"/>
+      <c r="H20" s="188"/>
       <c r="I20" s="37">
         <v>0</v>
       </c>
@@ -4770,16 +4802,16 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A25" s="206" t="s">
+      <c r="A25" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="172"/>
-      <c r="C25" s="172"/>
-      <c r="D25" s="173"/>
-      <c r="E25" s="174"/>
-      <c r="F25" s="175"/>
-      <c r="G25" s="176"/>
-      <c r="H25" s="177"/>
+      <c r="B25" s="183"/>
+      <c r="C25" s="183"/>
+      <c r="D25" s="184"/>
+      <c r="E25" s="185"/>
+      <c r="F25" s="186"/>
+      <c r="G25" s="187"/>
+      <c r="H25" s="188"/>
       <c r="I25" s="37">
         <v>1</v>
       </c>
@@ -4863,16 +4895,16 @@
       <c r="L27" s="34"/>
     </row>
     <row r="28" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A28" s="206" t="s">
+      <c r="A28" s="182" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="172"/>
-      <c r="C28" s="172"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="174"/>
-      <c r="F28" s="175"/>
-      <c r="G28" s="176"/>
-      <c r="H28" s="177"/>
+      <c r="B28" s="183"/>
+      <c r="C28" s="183"/>
+      <c r="D28" s="184"/>
+      <c r="E28" s="185"/>
+      <c r="F28" s="186"/>
+      <c r="G28" s="187"/>
+      <c r="H28" s="188"/>
       <c r="I28" s="37"/>
       <c r="J28" s="36">
         <f>J27+I28</f>
@@ -5201,10 +5233,10 @@
       <c r="L37" s="12"/>
     </row>
     <row r="38" spans="1:12" ht="21" customHeight="1">
-      <c r="A38" s="207"/>
-      <c r="B38" s="179"/>
-      <c r="C38" s="179"/>
-      <c r="D38" s="180"/>
+      <c r="A38" s="189"/>
+      <c r="B38" s="181"/>
+      <c r="C38" s="181"/>
+      <c r="D38" s="190"/>
       <c r="E38" s="12"/>
       <c r="F38" s="43"/>
       <c r="G38" s="44"/>
@@ -5215,37 +5247,37 @@
       <c r="L38" s="12"/>
     </row>
     <row r="39" spans="1:12" ht="101.25" customHeight="1">
-      <c r="A39" s="208" t="s">
+      <c r="A39" s="191" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="179"/>
-      <c r="C39" s="179"/>
-      <c r="D39" s="209"/>
-      <c r="E39" s="181"/>
-      <c r="F39" s="182"/>
-      <c r="G39" s="183"/>
-      <c r="H39" s="184"/>
+      <c r="B39" s="181"/>
+      <c r="C39" s="181"/>
+      <c r="D39" s="192"/>
+      <c r="E39" s="193"/>
+      <c r="F39" s="194"/>
+      <c r="G39" s="195"/>
+      <c r="H39" s="196"/>
       <c r="I39" s="39"/>
       <c r="J39" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="K39" s="203"/>
+      <c r="K39" s="178"/>
       <c r="L39" s="12"/>
     </row>
     <row r="40" spans="1:12" ht="145.5" customHeight="1">
-      <c r="A40" s="205" t="s">
+      <c r="A40" s="180" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="179"/>
-      <c r="C40" s="179"/>
-      <c r="D40" s="180"/>
-      <c r="E40" s="181"/>
-      <c r="F40" s="182"/>
-      <c r="G40" s="183"/>
-      <c r="H40" s="184"/>
+      <c r="B40" s="181"/>
+      <c r="C40" s="181"/>
+      <c r="D40" s="190"/>
+      <c r="E40" s="193"/>
+      <c r="F40" s="194"/>
+      <c r="G40" s="195"/>
+      <c r="H40" s="196"/>
       <c r="I40" s="39"/>
       <c r="J40" s="52"/>
-      <c r="K40" s="204"/>
+      <c r="K40" s="179"/>
     </row>
     <row r="41" spans="1:12" ht="12.75" customHeight="1">
       <c r="A41" s="28"/>
@@ -5586,6 +5618,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:H7"/>
     <mergeCell ref="K39:K40"/>
     <mergeCell ref="A40:C40"/>
     <mergeCell ref="A20:H20"/>
@@ -5594,12 +5632,6 @@
     <mergeCell ref="A38:D38"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="D39:H40"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B4:H7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5615,7 +5647,7 @@
   <dimension ref="A1:M72"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F9" sqref="F1:H1048576"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5637,108 +5669,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="198" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="181"/>
-      <c r="F1" s="182"/>
-      <c r="G1" s="183"/>
-      <c r="H1" s="184"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="190"/>
+      <c r="E1" s="193"/>
+      <c r="F1" s="194"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="196"/>
     </row>
     <row r="2" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A2" s="185" t="s">
+      <c r="A2" s="199" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="179"/>
-      <c r="C2" s="179"/>
-      <c r="D2" s="180"/>
-      <c r="E2" s="181"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="183"/>
-      <c r="H2" s="184"/>
+      <c r="B2" s="181"/>
+      <c r="C2" s="181"/>
+      <c r="D2" s="190"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="194"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="196"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A3" s="186" t="s">
+      <c r="A3" s="200" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="179"/>
-      <c r="C3" s="179"/>
-      <c r="D3" s="180"/>
-      <c r="E3" s="181"/>
-      <c r="F3" s="182"/>
-      <c r="G3" s="183"/>
-      <c r="H3" s="184"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="190"/>
+      <c r="E3" s="193"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="196"/>
       <c r="I3" s="35"/>
       <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A4" s="187" t="s">
+      <c r="A4" s="201" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="190" t="s">
+      <c r="B4" s="204" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="191"/>
-      <c r="D4" s="192"/>
-      <c r="E4" s="193"/>
-      <c r="F4" s="194"/>
-      <c r="G4" s="195"/>
-      <c r="H4" s="196"/>
+      <c r="C4" s="205"/>
+      <c r="D4" s="206"/>
+      <c r="E4" s="207"/>
+      <c r="F4" s="208"/>
+      <c r="G4" s="209"/>
+      <c r="H4" s="210"/>
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A5" s="188"/>
-      <c r="B5" s="191"/>
-      <c r="C5" s="191"/>
-      <c r="D5" s="192"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="194"/>
-      <c r="G5" s="195"/>
-      <c r="H5" s="196"/>
+      <c r="A5" s="202"/>
+      <c r="B5" s="205"/>
+      <c r="C5" s="205"/>
+      <c r="D5" s="206"/>
+      <c r="E5" s="207"/>
+      <c r="F5" s="208"/>
+      <c r="G5" s="209"/>
+      <c r="H5" s="210"/>
       <c r="I5" s="35"/>
       <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="22.5" hidden="1" customHeight="1">
-      <c r="A6" s="188"/>
-      <c r="B6" s="191"/>
-      <c r="C6" s="191"/>
-      <c r="D6" s="192"/>
-      <c r="E6" s="193"/>
-      <c r="F6" s="194"/>
-      <c r="G6" s="195"/>
-      <c r="H6" s="196"/>
+      <c r="A6" s="202"/>
+      <c r="B6" s="205"/>
+      <c r="C6" s="205"/>
+      <c r="D6" s="206"/>
+      <c r="E6" s="207"/>
+      <c r="F6" s="208"/>
+      <c r="G6" s="209"/>
+      <c r="H6" s="210"/>
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
     </row>
     <row r="7" spans="1:12" ht="10.5" hidden="1" customHeight="1">
-      <c r="A7" s="189"/>
-      <c r="B7" s="197"/>
-      <c r="C7" s="197"/>
-      <c r="D7" s="198"/>
-      <c r="E7" s="199"/>
-      <c r="F7" s="200"/>
-      <c r="G7" s="201"/>
-      <c r="H7" s="202"/>
+      <c r="A7" s="203"/>
+      <c r="B7" s="211"/>
+      <c r="C7" s="211"/>
+      <c r="D7" s="212"/>
+      <c r="E7" s="213"/>
+      <c r="F7" s="214"/>
+      <c r="G7" s="215"/>
+      <c r="H7" s="216"/>
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A8" s="171" t="s">
+      <c r="A8" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="172"/>
-      <c r="C8" s="172"/>
-      <c r="D8" s="173"/>
-      <c r="E8" s="174"/>
-      <c r="F8" s="175"/>
-      <c r="G8" s="176"/>
-      <c r="H8" s="177"/>
+      <c r="B8" s="183"/>
+      <c r="C8" s="183"/>
+      <c r="D8" s="184"/>
+      <c r="E8" s="185"/>
+      <c r="F8" s="186"/>
+      <c r="G8" s="187"/>
+      <c r="H8" s="188"/>
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
     </row>
@@ -6103,16 +6135,16 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A20" s="206" t="s">
+      <c r="A20" s="182" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="172"/>
-      <c r="C20" s="172"/>
-      <c r="D20" s="173"/>
-      <c r="E20" s="174"/>
-      <c r="F20" s="175"/>
-      <c r="G20" s="176"/>
-      <c r="H20" s="177"/>
+      <c r="B20" s="183"/>
+      <c r="C20" s="183"/>
+      <c r="D20" s="184"/>
+      <c r="E20" s="185"/>
+      <c r="F20" s="186"/>
+      <c r="G20" s="187"/>
+      <c r="H20" s="188"/>
       <c r="I20" s="37">
         <v>0</v>
       </c>
@@ -6254,16 +6286,16 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A25" s="206" t="s">
+      <c r="A25" s="182" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="172"/>
-      <c r="C25" s="172"/>
-      <c r="D25" s="173"/>
-      <c r="E25" s="174"/>
-      <c r="F25" s="175"/>
-      <c r="G25" s="176"/>
-      <c r="H25" s="177"/>
+      <c r="B25" s="183"/>
+      <c r="C25" s="183"/>
+      <c r="D25" s="184"/>
+      <c r="E25" s="185"/>
+      <c r="F25" s="186"/>
+      <c r="G25" s="187"/>
+      <c r="H25" s="188"/>
       <c r="I25" s="37">
         <v>1</v>
       </c>
@@ -6419,16 +6451,16 @@
       <c r="L29" s="34"/>
     </row>
     <row r="30" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A30" s="206" t="s">
+      <c r="A30" s="182" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="172"/>
-      <c r="C30" s="172"/>
-      <c r="D30" s="173"/>
-      <c r="E30" s="174"/>
-      <c r="F30" s="175"/>
-      <c r="G30" s="176"/>
-      <c r="H30" s="177"/>
+      <c r="B30" s="183"/>
+      <c r="C30" s="183"/>
+      <c r="D30" s="184"/>
+      <c r="E30" s="185"/>
+      <c r="F30" s="186"/>
+      <c r="G30" s="187"/>
+      <c r="H30" s="188"/>
       <c r="I30" s="37"/>
       <c r="J30" s="36">
         <f>J29+I30</f>
@@ -6794,10 +6826,10 @@
       <c r="L40" s="12"/>
     </row>
     <row r="41" spans="1:12" ht="21" customHeight="1">
-      <c r="A41" s="207"/>
-      <c r="B41" s="179"/>
-      <c r="C41" s="179"/>
-      <c r="D41" s="180"/>
+      <c r="A41" s="189"/>
+      <c r="B41" s="181"/>
+      <c r="C41" s="181"/>
+      <c r="D41" s="190"/>
       <c r="E41" s="12"/>
       <c r="F41" s="43"/>
       <c r="G41" s="44"/>
@@ -6808,37 +6840,37 @@
       <c r="L41" s="12"/>
     </row>
     <row r="42" spans="1:12" ht="101.25" customHeight="1">
-      <c r="A42" s="208" t="s">
+      <c r="A42" s="191" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="179"/>
-      <c r="C42" s="179"/>
-      <c r="D42" s="209"/>
-      <c r="E42" s="181"/>
-      <c r="F42" s="182"/>
-      <c r="G42" s="183"/>
-      <c r="H42" s="184"/>
+      <c r="B42" s="181"/>
+      <c r="C42" s="181"/>
+      <c r="D42" s="192"/>
+      <c r="E42" s="193"/>
+      <c r="F42" s="194"/>
+      <c r="G42" s="195"/>
+      <c r="H42" s="196"/>
       <c r="I42" s="39"/>
       <c r="J42" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="K42" s="203"/>
+      <c r="K42" s="178"/>
       <c r="L42" s="12"/>
     </row>
     <row r="43" spans="1:12" ht="145.5" customHeight="1">
-      <c r="A43" s="205" t="s">
+      <c r="A43" s="180" t="s">
         <v>64</v>
       </c>
-      <c r="B43" s="179"/>
-      <c r="C43" s="179"/>
-      <c r="D43" s="180"/>
-      <c r="E43" s="181"/>
-      <c r="F43" s="182"/>
-      <c r="G43" s="183"/>
-      <c r="H43" s="184"/>
+      <c r="B43" s="181"/>
+      <c r="C43" s="181"/>
+      <c r="D43" s="190"/>
+      <c r="E43" s="193"/>
+      <c r="F43" s="194"/>
+      <c r="G43" s="195"/>
+      <c r="H43" s="196"/>
       <c r="I43" s="39"/>
       <c r="J43" s="52"/>
-      <c r="K43" s="204"/>
+      <c r="K43" s="179"/>
     </row>
     <row r="44" spans="1:12" ht="12.75" customHeight="1">
       <c r="A44" s="28"/>
@@ -7179,6 +7211,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:H7"/>
     <mergeCell ref="K42:K43"/>
     <mergeCell ref="A43:C43"/>
     <mergeCell ref="A20:H20"/>
@@ -7187,12 +7225,6 @@
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="D42:H43"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B4:H7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7201,6 +7233,1708 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1BDE0D-D84C-4B87-858B-77CB3AB9A19A}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="171" customWidth="1"/>
+    <col min="3" max="3" width="77.7109375" style="171" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="172" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="173" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="174" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="175" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="176" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" style="177" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="177" customWidth="1"/>
+    <col min="11" max="11" width="20" style="177" customWidth="1"/>
+    <col min="12" max="12" width="21" style="171" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="12" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="71.25" customHeight="1">
+      <c r="A1" s="198" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="190"/>
+      <c r="E1" s="193"/>
+      <c r="F1" s="194"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="196"/>
+    </row>
+    <row r="2" spans="1:12" ht="22.5" customHeight="1">
+      <c r="A2" s="199" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="181"/>
+      <c r="C2" s="181"/>
+      <c r="D2" s="190"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="194"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="196"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+    </row>
+    <row r="3" spans="1:12" ht="22.5" customHeight="1">
+      <c r="A3" s="200" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="181"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="190"/>
+      <c r="E3" s="193"/>
+      <c r="F3" s="194"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="196"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+    </row>
+    <row r="4" spans="1:12" ht="22.5" customHeight="1">
+      <c r="A4" s="201" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="204" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="205"/>
+      <c r="D4" s="206"/>
+      <c r="E4" s="207"/>
+      <c r="F4" s="208"/>
+      <c r="G4" s="209"/>
+      <c r="H4" s="210"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+    </row>
+    <row r="5" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
+      <c r="A5" s="202"/>
+      <c r="B5" s="205"/>
+      <c r="C5" s="205"/>
+      <c r="D5" s="206"/>
+      <c r="E5" s="207"/>
+      <c r="F5" s="208"/>
+      <c r="G5" s="209"/>
+      <c r="H5" s="210"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+    </row>
+    <row r="6" spans="1:12" ht="22.5" hidden="1" customHeight="1">
+      <c r="A6" s="202"/>
+      <c r="B6" s="205"/>
+      <c r="C6" s="205"/>
+      <c r="D6" s="206"/>
+      <c r="E6" s="207"/>
+      <c r="F6" s="208"/>
+      <c r="G6" s="209"/>
+      <c r="H6" s="210"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+    </row>
+    <row r="7" spans="1:12" ht="10.5" hidden="1" customHeight="1">
+      <c r="A7" s="203"/>
+      <c r="B7" s="211"/>
+      <c r="C7" s="211"/>
+      <c r="D7" s="212"/>
+      <c r="E7" s="213"/>
+      <c r="F7" s="214"/>
+      <c r="G7" s="215"/>
+      <c r="H7" s="216"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+    </row>
+    <row r="8" spans="1:12" ht="33.75" customHeight="1" thickBot="1">
+      <c r="A8" s="197" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="183"/>
+      <c r="C8" s="183"/>
+      <c r="D8" s="184"/>
+      <c r="E8" s="185"/>
+      <c r="F8" s="186"/>
+      <c r="G8" s="187"/>
+      <c r="H8" s="188"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+    </row>
+    <row r="9" spans="1:12" ht="42.75" customHeight="1" thickBot="1">
+      <c r="A9" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="123" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="170" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="124" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="37">
+        <v>1</v>
+      </c>
+      <c r="J9" s="36">
+        <v>0.77777777777777801</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="24" customHeight="1">
+      <c r="A10" s="20">
+        <f t="shared" ref="A10:A19" si="0">J9</f>
+        <v>0.77777777777777801</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="147" t="str">
+        <f>Roles!B2</f>
+        <v>Davie</v>
+      </c>
+      <c r="E10" s="22">
+        <v>20</v>
+      </c>
+      <c r="F10" s="148"/>
+      <c r="G10" s="149"/>
+      <c r="H10" s="150"/>
+      <c r="I10" s="37">
+        <v>1.0138888888888888</v>
+      </c>
+      <c r="J10" s="36">
+        <f t="shared" ref="J10:J41" si="1">J9+I10</f>
+        <v>1.791666666666667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="24" customHeight="1">
+      <c r="A11" s="20">
+        <f t="shared" si="0"/>
+        <v>1.791666666666667</v>
+      </c>
+      <c r="B11" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="69" t="s">
+        <v>330</v>
+      </c>
+      <c r="D11" s="99" t="str">
+        <f>Roles!B3</f>
+        <v>Harper</v>
+      </c>
+      <c r="E11" s="76">
+        <v>4</v>
+      </c>
+      <c r="F11" s="151"/>
+      <c r="G11" s="152" t="s">
+        <v>331</v>
+      </c>
+      <c r="H11" s="153" t="s">
+        <v>332</v>
+      </c>
+      <c r="I11" s="37">
+        <v>5.0027777777777782</v>
+      </c>
+      <c r="J11" s="36">
+        <f t="shared" si="1"/>
+        <v>6.7944444444444452</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="24" customHeight="1">
+      <c r="A12" s="20">
+        <f t="shared" si="0"/>
+        <v>6.7944444444444452</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>333</v>
+      </c>
+      <c r="C12" s="70" t="s">
+        <v>334</v>
+      </c>
+      <c r="D12" s="99" t="str">
+        <f>Roles!B2</f>
+        <v>Davie</v>
+      </c>
+      <c r="E12" s="76">
+        <v>5</v>
+      </c>
+      <c r="F12" s="151" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="152" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="153" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="37">
+        <v>0</v>
+      </c>
+      <c r="J12" s="36">
+        <f t="shared" si="1"/>
+        <v>6.7944444444444452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="24" customHeight="1">
+      <c r="A13" s="20">
+        <f t="shared" si="0"/>
+        <v>6.7944444444444452</v>
+      </c>
+      <c r="B13" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="73" t="s">
+        <v>335</v>
+      </c>
+      <c r="D13" s="99" t="str">
+        <f>Roles!B4</f>
+        <v>Harper</v>
+      </c>
+      <c r="E13" s="76">
+        <v>5</v>
+      </c>
+      <c r="F13" s="151">
+        <v>3</v>
+      </c>
+      <c r="G13" s="152">
+        <v>4</v>
+      </c>
+      <c r="H13" s="153">
+        <v>5</v>
+      </c>
+      <c r="I13" s="37">
+        <v>1.0034722222222201</v>
+      </c>
+      <c r="J13" s="36">
+        <f t="shared" si="1"/>
+        <v>7.7979166666666657</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="24" customHeight="1">
+      <c r="A14" s="20">
+        <f t="shared" si="0"/>
+        <v>7.7979166666666657</v>
+      </c>
+      <c r="B14" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="73" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="99" t="str">
+        <f>Roles!B5</f>
+        <v>Bonnie Wang</v>
+      </c>
+      <c r="E14" s="76">
+        <v>1</v>
+      </c>
+      <c r="F14" s="151"/>
+      <c r="G14" s="152"/>
+      <c r="H14" s="153" t="s">
+        <v>336</v>
+      </c>
+      <c r="I14" s="37">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="J14" s="36">
+        <f t="shared" si="1"/>
+        <v>7.7986111111111098</v>
+      </c>
+      <c r="K14" s="36"/>
+      <c r="L14" s="34"/>
+    </row>
+    <row r="15" spans="1:12" ht="24.75" customHeight="1">
+      <c r="A15" s="20">
+        <f t="shared" si="0"/>
+        <v>7.7986111111111098</v>
+      </c>
+      <c r="B15" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="99" t="str">
+        <f>Roles!B8</f>
+        <v>Serena</v>
+      </c>
+      <c r="E15" s="76">
+        <v>1</v>
+      </c>
+      <c r="F15" s="151"/>
+      <c r="G15" s="152"/>
+      <c r="H15" s="153">
+        <v>1</v>
+      </c>
+      <c r="I15" s="37">
+        <v>1.0006944444444399</v>
+      </c>
+      <c r="J15" s="36">
+        <f t="shared" si="1"/>
+        <v>8.7993055555555504</v>
+      </c>
+      <c r="K15" s="36"/>
+      <c r="L15" s="34"/>
+    </row>
+    <row r="16" spans="1:12" ht="24" customHeight="1">
+      <c r="A16" s="20">
+        <f t="shared" si="0"/>
+        <v>8.7993055555555504</v>
+      </c>
+      <c r="B16" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="99" t="str">
+        <f>Roles!B9</f>
+        <v>Raymond Li</v>
+      </c>
+      <c r="E16" s="76">
+        <v>1</v>
+      </c>
+      <c r="F16" s="151"/>
+      <c r="G16" s="152"/>
+      <c r="H16" s="153">
+        <v>1</v>
+      </c>
+      <c r="I16" s="37">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="J16" s="36">
+        <f t="shared" si="1"/>
+        <v>8.7999999999999954</v>
+      </c>
+      <c r="K16" s="36"/>
+      <c r="L16" s="34"/>
+    </row>
+    <row r="17" spans="1:12" ht="24" customHeight="1">
+      <c r="A17" s="20">
+        <f t="shared" si="0"/>
+        <v>8.7999999999999954</v>
+      </c>
+      <c r="B17" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="99" t="str">
+        <f>Roles!B10</f>
+        <v>Raven</v>
+      </c>
+      <c r="E17" s="76">
+        <v>2</v>
+      </c>
+      <c r="F17" s="151"/>
+      <c r="G17" s="152" t="s">
+        <v>336</v>
+      </c>
+      <c r="H17" s="153">
+        <v>2</v>
+      </c>
+      <c r="I17" s="37">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="J17" s="36">
+        <f t="shared" si="1"/>
+        <v>8.8013888888888836</v>
+      </c>
+      <c r="K17" s="36"/>
+      <c r="L17" s="34"/>
+    </row>
+    <row r="18" spans="1:12" ht="24" customHeight="1">
+      <c r="A18" s="20">
+        <f t="shared" si="0"/>
+        <v>8.8013888888888836</v>
+      </c>
+      <c r="B18" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="99" t="str">
+        <f>Roles!B5</f>
+        <v>Bonnie Wang</v>
+      </c>
+      <c r="E18" s="76">
+        <v>1</v>
+      </c>
+      <c r="F18" s="151"/>
+      <c r="G18" s="152"/>
+      <c r="H18" s="153">
+        <v>1</v>
+      </c>
+      <c r="I18" s="37">
+        <v>0</v>
+      </c>
+      <c r="J18" s="36">
+        <f t="shared" si="1"/>
+        <v>8.8013888888888836</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="24" customHeight="1" thickBot="1">
+      <c r="A19" s="125">
+        <f t="shared" si="0"/>
+        <v>8.8013888888888836</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>337</v>
+      </c>
+      <c r="D19" s="99" t="str">
+        <f>Roles!B4</f>
+        <v>Harper</v>
+      </c>
+      <c r="E19" s="127">
+        <v>1</v>
+      </c>
+      <c r="F19" s="154"/>
+      <c r="G19" s="155"/>
+      <c r="H19" s="156">
+        <v>1</v>
+      </c>
+      <c r="I19" s="37">
+        <v>6.9444444444444404E-4</v>
+      </c>
+      <c r="J19" s="36">
+        <f t="shared" si="1"/>
+        <v>8.8020833333333286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="24" customHeight="1" thickBot="1">
+      <c r="A20" s="182" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="183"/>
+      <c r="C20" s="183"/>
+      <c r="D20" s="184"/>
+      <c r="E20" s="185"/>
+      <c r="F20" s="186"/>
+      <c r="G20" s="187"/>
+      <c r="H20" s="188"/>
+      <c r="I20" s="37">
+        <v>0</v>
+      </c>
+      <c r="J20" s="36">
+        <f t="shared" si="1"/>
+        <v>8.8020833333333286</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="24" customHeight="1">
+      <c r="A21" s="20">
+        <f>J20</f>
+        <v>8.8020833333333286</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="98" t="str">
+        <f>Roles!B6</f>
+        <v>Elliot Zhang</v>
+      </c>
+      <c r="E21" s="27">
+        <v>20</v>
+      </c>
+      <c r="F21" s="128">
+        <v>1</v>
+      </c>
+      <c r="G21" s="101">
+        <v>1.5</v>
+      </c>
+      <c r="H21" s="102">
+        <v>2</v>
+      </c>
+      <c r="I21" s="37">
+        <v>1.388888888888889E-2</v>
+      </c>
+      <c r="J21" s="36">
+        <f t="shared" si="1"/>
+        <v>8.8159722222222179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="24" customHeight="1">
+      <c r="A22" s="20">
+        <f>J21</f>
+        <v>8.8159722222222179</v>
+      </c>
+      <c r="B22" s="70" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="99" t="str">
+        <f>Roles!B7</f>
+        <v>Julia Zhu</v>
+      </c>
+      <c r="E22" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="103" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="104" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="105" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="37">
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="J22" s="36">
+        <f t="shared" si="1"/>
+        <v>8.8201388888888843</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="24" customHeight="1">
+      <c r="A23" s="20">
+        <f>J22</f>
+        <v>8.8201388888888843</v>
+      </c>
+      <c r="B23" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="99" t="str">
+        <f>Roles!B4</f>
+        <v>Harper</v>
+      </c>
+      <c r="E23" s="76">
+        <v>1</v>
+      </c>
+      <c r="F23" s="106"/>
+      <c r="G23" s="107">
+        <v>0.5</v>
+      </c>
+      <c r="H23" s="108">
+        <v>1</v>
+      </c>
+      <c r="I23" s="37">
+        <v>6.9444444444444404E-4</v>
+      </c>
+      <c r="J23" s="36">
+        <f t="shared" si="1"/>
+        <v>8.8208333333333293</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="24" customHeight="1" thickBot="1">
+      <c r="A24" s="129">
+        <f>J23</f>
+        <v>8.8208333333333293</v>
+      </c>
+      <c r="B24" s="130" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="131"/>
+      <c r="D24" s="126" t="str">
+        <f>Roles!B4</f>
+        <v>Harper</v>
+      </c>
+      <c r="E24" s="132">
+        <v>7</v>
+      </c>
+      <c r="F24" s="133"/>
+      <c r="G24" s="134"/>
+      <c r="H24" s="135" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="37">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="J24" s="36">
+        <f t="shared" si="1"/>
+        <v>8.8256944444444407</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="24" customHeight="1" thickBot="1">
+      <c r="A25" s="182" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="183"/>
+      <c r="C25" s="183"/>
+      <c r="D25" s="184"/>
+      <c r="E25" s="185"/>
+      <c r="F25" s="186"/>
+      <c r="G25" s="187"/>
+      <c r="H25" s="188"/>
+      <c r="I25" s="37">
+        <v>1</v>
+      </c>
+      <c r="J25" s="36">
+        <f t="shared" si="1"/>
+        <v>9.8256944444444407</v>
+      </c>
+      <c r="K25" s="36"/>
+      <c r="L25" s="34"/>
+    </row>
+    <row r="26" spans="1:12" ht="24" customHeight="1">
+      <c r="A26" s="20">
+        <f t="shared" ref="A26:A27" si="2">J25</f>
+        <v>9.8256944444444407</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="98" t="str">
+        <f>Roles!B4</f>
+        <v>Harper</v>
+      </c>
+      <c r="E26" s="27">
+        <v>1</v>
+      </c>
+      <c r="F26" s="100"/>
+      <c r="G26" s="101">
+        <v>0.5</v>
+      </c>
+      <c r="H26" s="102">
+        <v>1</v>
+      </c>
+      <c r="I26" s="37">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="J26" s="36">
+        <f t="shared" si="1"/>
+        <v>9.8263888888888857</v>
+      </c>
+      <c r="K26" s="36"/>
+      <c r="L26" s="34"/>
+    </row>
+    <row r="27" spans="1:12" ht="47.25" customHeight="1">
+      <c r="A27" s="20">
+        <f t="shared" si="2"/>
+        <v>9.8263888888888857</v>
+      </c>
+      <c r="B27" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="74" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="113" t="str">
+        <f>Roles!B11</f>
+        <v>Jill Chen</v>
+      </c>
+      <c r="E27" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="103" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="104" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" s="105" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27" s="37">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="J27" s="36">
+        <f t="shared" si="1"/>
+        <v>9.8312499999999972</v>
+      </c>
+      <c r="K27" s="36"/>
+      <c r="L27" s="34"/>
+    </row>
+    <row r="28" spans="1:12" ht="24" customHeight="1">
+      <c r="A28" s="20">
+        <f>J27</f>
+        <v>9.8312499999999972</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="113" t="str">
+        <f>Roles!B4</f>
+        <v>Harper</v>
+      </c>
+      <c r="E28" s="27">
+        <v>1</v>
+      </c>
+      <c r="F28" s="100"/>
+      <c r="G28" s="101">
+        <v>0.5</v>
+      </c>
+      <c r="H28" s="102">
+        <v>1</v>
+      </c>
+      <c r="I28" s="37">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="J28" s="36">
+        <f>J27+I28</f>
+        <v>9.8319444444444422</v>
+      </c>
+      <c r="K28" s="36"/>
+      <c r="L28" s="34"/>
+    </row>
+    <row r="29" spans="1:12" ht="18">
+      <c r="A29" s="20">
+        <f>J28</f>
+        <v>9.8319444444444422</v>
+      </c>
+      <c r="B29" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="114" t="str">
+        <f>Roles!B12</f>
+        <v>Rice Fan</v>
+      </c>
+      <c r="E29" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="103" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="104" t="s">
+        <v>35</v>
+      </c>
+      <c r="H29" s="105" t="s">
+        <v>42</v>
+      </c>
+      <c r="I29" s="37">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="J29" s="36">
+        <f>J28+I29</f>
+        <v>9.8368055555555536</v>
+      </c>
+      <c r="K29" s="36"/>
+      <c r="L29" s="34"/>
+    </row>
+    <row r="30" spans="1:12" ht="18">
+      <c r="A30" s="20">
+        <f>J29</f>
+        <v>9.8368055555555536</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>359</v>
+      </c>
+      <c r="D30" s="113" t="str">
+        <f>Roles!B4</f>
+        <v>Harper</v>
+      </c>
+      <c r="E30" s="27">
+        <v>1</v>
+      </c>
+      <c r="F30" s="100"/>
+      <c r="G30" s="101">
+        <v>0.5</v>
+      </c>
+      <c r="H30" s="102">
+        <v>1</v>
+      </c>
+      <c r="I30" s="37">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="J30" s="36">
+        <f>J29+I30</f>
+        <v>9.8374999999999986</v>
+      </c>
+      <c r="K30" s="36"/>
+      <c r="L30" s="34"/>
+    </row>
+    <row r="31" spans="1:12" ht="18.75" thickBot="1">
+      <c r="A31" s="20">
+        <f>J30</f>
+        <v>9.8374999999999986</v>
+      </c>
+      <c r="B31" s="73" t="s">
+        <v>361</v>
+      </c>
+      <c r="C31" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="114" t="str">
+        <f>Roles!B13</f>
+        <v>Karen</v>
+      </c>
+      <c r="E31" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="103" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="104" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" s="105" t="s">
+        <v>42</v>
+      </c>
+      <c r="I31" s="37">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="J31" s="36">
+        <f>J30+I31</f>
+        <v>9.84236111111111</v>
+      </c>
+      <c r="K31" s="36"/>
+      <c r="L31" s="34"/>
+    </row>
+    <row r="32" spans="1:12" ht="24" customHeight="1" thickBot="1">
+      <c r="A32" s="182" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="183"/>
+      <c r="C32" s="183"/>
+      <c r="D32" s="184"/>
+      <c r="E32" s="185"/>
+      <c r="F32" s="186"/>
+      <c r="G32" s="187"/>
+      <c r="H32" s="188"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="36">
+        <f>J31+I32</f>
+        <v>9.84236111111111</v>
+      </c>
+      <c r="K32" s="36"/>
+      <c r="L32" s="34"/>
+    </row>
+    <row r="33" spans="1:12" ht="24" customHeight="1">
+      <c r="A33" s="20">
+        <f>J32</f>
+        <v>9.84236111111111</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="98" t="str">
+        <f>Roles!B5</f>
+        <v>Bonnie Wang</v>
+      </c>
+      <c r="E33" s="27">
+        <v>1</v>
+      </c>
+      <c r="F33" s="148"/>
+      <c r="G33" s="149">
+        <v>0.5</v>
+      </c>
+      <c r="H33" s="150">
+        <v>1</v>
+      </c>
+      <c r="I33" s="37">
+        <v>1.0006944444444399</v>
+      </c>
+      <c r="J33" s="36">
+        <f t="shared" si="1"/>
+        <v>10.84305555555555</v>
+      </c>
+      <c r="K33" s="36"/>
+      <c r="L33" s="34"/>
+    </row>
+    <row r="34" spans="1:12" ht="24" customHeight="1">
+      <c r="A34" s="20">
+        <f>J33</f>
+        <v>10.84305555555555</v>
+      </c>
+      <c r="B34" s="55" t="s">
+        <v>338</v>
+      </c>
+      <c r="C34" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="98" t="str">
+        <f>Roles!B15</f>
+        <v>Qiyang Li</v>
+      </c>
+      <c r="E34" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" s="151">
+        <v>2</v>
+      </c>
+      <c r="G34" s="152">
+        <v>2.5</v>
+      </c>
+      <c r="H34" s="153">
+        <v>3</v>
+      </c>
+      <c r="I34" s="37">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="J34" s="36">
+        <f t="shared" si="1"/>
+        <v>10.845138888888883</v>
+      </c>
+      <c r="K34" s="36"/>
+      <c r="L34" s="34"/>
+    </row>
+    <row r="35" spans="1:12" ht="24" customHeight="1">
+      <c r="A35" s="20">
+        <f>J34</f>
+        <v>10.845138888888883</v>
+      </c>
+      <c r="B35" s="55" t="s">
+        <v>288</v>
+      </c>
+      <c r="C35" s="56" t="s">
+        <v>356</v>
+      </c>
+      <c r="D35" s="98" t="str">
+        <f>Roles!B16</f>
+        <v>Olivia Wang</v>
+      </c>
+      <c r="E35" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="151">
+        <v>2</v>
+      </c>
+      <c r="G35" s="152">
+        <v>2.5</v>
+      </c>
+      <c r="H35" s="153">
+        <v>3</v>
+      </c>
+      <c r="I35" s="37">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="J35" s="36">
+        <f t="shared" si="1"/>
+        <v>10.847222222222216</v>
+      </c>
+      <c r="K35" s="36"/>
+      <c r="L35" s="34"/>
+    </row>
+    <row r="36" spans="1:12" ht="24" customHeight="1">
+      <c r="A36" s="20">
+        <f>J35</f>
+        <v>10.847222222222216</v>
+      </c>
+      <c r="B36" s="55" t="s">
+        <v>297</v>
+      </c>
+      <c r="C36" s="56" t="s">
+        <v>360</v>
+      </c>
+      <c r="D36" s="98" t="str">
+        <f>Roles!B17</f>
+        <v>Nancy</v>
+      </c>
+      <c r="E36" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="151">
+        <v>2</v>
+      </c>
+      <c r="G36" s="152">
+        <v>2.5</v>
+      </c>
+      <c r="H36" s="153">
+        <v>3</v>
+      </c>
+      <c r="I36" s="37">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="J36" s="36">
+        <f t="shared" ref="J36" si="3">J35+I36</f>
+        <v>10.849305555555549</v>
+      </c>
+      <c r="K36" s="36"/>
+      <c r="L36" s="34"/>
+    </row>
+    <row r="37" spans="1:12" ht="24" customHeight="1">
+      <c r="A37" s="20">
+        <f>J36</f>
+        <v>10.849305555555549</v>
+      </c>
+      <c r="B37" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="99" t="str">
+        <f>Roles!B9</f>
+        <v>Raymond Li</v>
+      </c>
+      <c r="E37" s="75" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="151"/>
+      <c r="G37" s="152">
+        <v>1.5</v>
+      </c>
+      <c r="H37" s="153">
+        <v>2</v>
+      </c>
+      <c r="I37" s="37">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="J37" s="36">
+        <f>J36+I37</f>
+        <v>10.850694444444438</v>
+      </c>
+      <c r="K37" s="36"/>
+      <c r="L37" s="38"/>
+    </row>
+    <row r="38" spans="1:12" ht="24" customHeight="1">
+      <c r="A38" s="20">
+        <f t="shared" ref="A38:A41" si="4">J37</f>
+        <v>10.850694444444438</v>
+      </c>
+      <c r="B38" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="99" t="str">
+        <f>Roles!B10</f>
+        <v>Raven</v>
+      </c>
+      <c r="E38" s="75" t="s">
+        <v>53</v>
+      </c>
+      <c r="F38" s="151">
+        <v>2</v>
+      </c>
+      <c r="G38" s="152">
+        <v>2.5</v>
+      </c>
+      <c r="H38" s="153">
+        <v>3</v>
+      </c>
+      <c r="I38" s="37">
+        <v>2.0833333333333329E-3</v>
+      </c>
+      <c r="J38" s="36">
+        <f t="shared" si="1"/>
+        <v>10.852777777777771</v>
+      </c>
+      <c r="K38" s="36"/>
+      <c r="L38" s="38"/>
+    </row>
+    <row r="39" spans="1:12" ht="24" customHeight="1">
+      <c r="A39" s="20">
+        <f t="shared" si="4"/>
+        <v>10.852777777777771</v>
+      </c>
+      <c r="B39" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="99" t="str">
+        <f>Roles!B8</f>
+        <v>Serena</v>
+      </c>
+      <c r="E39" s="75" t="s">
+        <v>51</v>
+      </c>
+      <c r="F39" s="151"/>
+      <c r="G39" s="152">
+        <v>1.5</v>
+      </c>
+      <c r="H39" s="153">
+        <v>2</v>
+      </c>
+      <c r="I39" s="37">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="J39" s="36">
+        <f t="shared" si="1"/>
+        <v>10.854166666666659</v>
+      </c>
+      <c r="K39" s="36"/>
+      <c r="L39" s="38"/>
+    </row>
+    <row r="40" spans="1:12" ht="24" customHeight="1">
+      <c r="A40" s="20">
+        <f t="shared" si="4"/>
+        <v>10.854166666666659</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="157" t="s">
+        <v>340</v>
+      </c>
+      <c r="D40" s="99" t="str">
+        <f>Roles!B2</f>
+        <v>Davie</v>
+      </c>
+      <c r="E40" s="76">
+        <v>1</v>
+      </c>
+      <c r="F40" s="151"/>
+      <c r="G40" s="152"/>
+      <c r="H40" s="153">
+        <v>1</v>
+      </c>
+      <c r="I40" s="37">
+        <v>6.9444444444444404E-4</v>
+      </c>
+      <c r="J40" s="36">
+        <f t="shared" si="1"/>
+        <v>10.854861111111104</v>
+      </c>
+      <c r="K40" s="36"/>
+      <c r="L40" s="38"/>
+    </row>
+    <row r="41" spans="1:12" ht="24" customHeight="1">
+      <c r="A41" s="20">
+        <f t="shared" si="4"/>
+        <v>10.854861111111104</v>
+      </c>
+      <c r="B41" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="99" t="str">
+        <f>Roles!B5</f>
+        <v>Bonnie Wang</v>
+      </c>
+      <c r="E41" s="75" t="s">
+        <v>341</v>
+      </c>
+      <c r="F41" s="151" t="s">
+        <v>342</v>
+      </c>
+      <c r="G41" s="152" t="s">
+        <v>332</v>
+      </c>
+      <c r="H41" s="153" t="s">
+        <v>343</v>
+      </c>
+      <c r="I41" s="37">
+        <v>1.0034722222222223</v>
+      </c>
+      <c r="J41" s="36">
+        <f t="shared" si="1"/>
+        <v>11.858333333333327</v>
+      </c>
+      <c r="K41" s="36"/>
+      <c r="L41" s="38"/>
+    </row>
+    <row r="42" spans="1:12" ht="24" customHeight="1" thickBot="1">
+      <c r="A42" s="77">
+        <f>J41</f>
+        <v>11.858333333333327</v>
+      </c>
+      <c r="B42" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="73" t="s">
+        <v>344</v>
+      </c>
+      <c r="D42" s="99" t="str">
+        <f>Roles!B4</f>
+        <v>Harper</v>
+      </c>
+      <c r="E42" s="75" t="s">
+        <v>56</v>
+      </c>
+      <c r="F42" s="158" t="s">
+        <v>57</v>
+      </c>
+      <c r="G42" s="159" t="s">
+        <v>58</v>
+      </c>
+      <c r="H42" s="160" t="s">
+        <v>56</v>
+      </c>
+      <c r="I42" s="37">
+        <v>1.0013888888888891</v>
+      </c>
+      <c r="J42" s="36">
+        <f>J41+I42</f>
+        <v>12.859722222222217</v>
+      </c>
+      <c r="K42" s="36"/>
+      <c r="L42" s="38"/>
+    </row>
+    <row r="43" spans="1:12" ht="24" customHeight="1" thickBot="1">
+      <c r="A43" s="77">
+        <f>J42</f>
+        <v>12.859722222222217</v>
+      </c>
+      <c r="B43" s="78" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="122" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="99" t="str">
+        <f>Roles!B3</f>
+        <v>Harper</v>
+      </c>
+      <c r="E43" s="71">
+        <v>2</v>
+      </c>
+      <c r="F43" s="109"/>
+      <c r="G43" s="110"/>
+      <c r="H43" s="111" t="s">
+        <v>56</v>
+      </c>
+      <c r="I43" s="37">
+        <v>1.0013888888888889</v>
+      </c>
+      <c r="J43" s="36">
+        <f>J41+I43</f>
+        <v>12.859722222222215</v>
+      </c>
+      <c r="K43" s="39"/>
+      <c r="L43" s="12"/>
+    </row>
+    <row r="44" spans="1:12" ht="21" customHeight="1">
+      <c r="A44" s="189"/>
+      <c r="B44" s="181"/>
+      <c r="C44" s="181"/>
+      <c r="D44" s="190"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="12"/>
+    </row>
+    <row r="45" spans="1:12" ht="101.25" customHeight="1">
+      <c r="A45" s="191" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="181"/>
+      <c r="C45" s="181"/>
+      <c r="D45" s="192"/>
+      <c r="E45" s="193"/>
+      <c r="F45" s="194"/>
+      <c r="G45" s="195"/>
+      <c r="H45" s="196"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="K45" s="178"/>
+      <c r="L45" s="12"/>
+    </row>
+    <row r="46" spans="1:12" ht="145.5" customHeight="1">
+      <c r="A46" s="180" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="181"/>
+      <c r="C46" s="181"/>
+      <c r="D46" s="190"/>
+      <c r="E46" s="193"/>
+      <c r="F46" s="194"/>
+      <c r="G46" s="195"/>
+      <c r="H46" s="196"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="52"/>
+      <c r="K46" s="179"/>
+    </row>
+    <row r="47" spans="1:12" ht="12.75" customHeight="1">
+      <c r="A47" s="28"/>
+      <c r="B47" s="12"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+    </row>
+    <row r="48" spans="1:12" ht="12.75" customHeight="1">
+      <c r="A48" s="28"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="29"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="46"/>
+    </row>
+    <row r="49" spans="1:13" ht="12.75" customHeight="1">
+      <c r="A49" s="28"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="48"/>
+    </row>
+    <row r="50" spans="1:13" ht="12.75" customHeight="1">
+      <c r="A50" s="28"/>
+      <c r="B50" s="12"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="33"/>
+      <c r="L50" s="177"/>
+    </row>
+    <row r="51" spans="1:13" ht="12.75" customHeight="1">
+      <c r="A51" s="28"/>
+      <c r="B51" s="12"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="33"/>
+      <c r="L51" s="177"/>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="28"/>
+      <c r="B52" s="12"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="33"/>
+      <c r="L52" s="177"/>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="28"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="33"/>
+      <c r="L53" s="177"/>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="28"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="33"/>
+      <c r="L54" s="177"/>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="28"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="E55" s="33"/>
+      <c r="L55" s="177"/>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="28"/>
+      <c r="B56" s="12"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="33"/>
+    </row>
+    <row r="57" spans="1:13" s="174" customFormat="1">
+      <c r="A57" s="28"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="33"/>
+      <c r="G57" s="175"/>
+      <c r="H57" s="176"/>
+      <c r="I57" s="177"/>
+      <c r="J57" s="177"/>
+      <c r="K57" s="177"/>
+      <c r="L57" s="171"/>
+      <c r="M57" s="12"/>
+    </row>
+    <row r="58" spans="1:13" s="174" customFormat="1">
+      <c r="A58" s="28"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="171"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="33"/>
+      <c r="G58" s="175"/>
+      <c r="H58" s="176"/>
+      <c r="I58" s="177"/>
+      <c r="J58" s="177"/>
+      <c r="K58" s="177"/>
+      <c r="L58" s="171"/>
+      <c r="M58" s="12"/>
+    </row>
+    <row r="59" spans="1:13" s="174" customFormat="1">
+      <c r="A59" s="28"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="32"/>
+      <c r="E59" s="33"/>
+      <c r="G59" s="175"/>
+      <c r="H59" s="176"/>
+      <c r="I59" s="177"/>
+      <c r="J59" s="177"/>
+      <c r="K59" s="177"/>
+      <c r="L59" s="171"/>
+      <c r="M59" s="12"/>
+    </row>
+    <row r="60" spans="1:13" s="174" customFormat="1">
+      <c r="A60" s="28"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="33"/>
+      <c r="G60" s="175"/>
+      <c r="H60" s="176"/>
+      <c r="I60" s="177"/>
+      <c r="J60" s="177"/>
+      <c r="K60" s="177"/>
+      <c r="L60" s="171"/>
+      <c r="M60" s="12"/>
+    </row>
+    <row r="61" spans="1:13" s="174" customFormat="1">
+      <c r="A61" s="28"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="33"/>
+      <c r="G61" s="175"/>
+      <c r="H61" s="176"/>
+      <c r="I61" s="177"/>
+      <c r="J61" s="177"/>
+      <c r="K61" s="177"/>
+      <c r="L61" s="171"/>
+      <c r="M61" s="12"/>
+    </row>
+    <row r="62" spans="1:13" s="174" customFormat="1">
+      <c r="A62" s="28"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="32"/>
+      <c r="E62" s="33"/>
+      <c r="G62" s="175"/>
+      <c r="H62" s="176"/>
+      <c r="I62" s="177"/>
+      <c r="J62" s="177"/>
+      <c r="K62" s="177"/>
+      <c r="L62" s="171"/>
+      <c r="M62" s="12"/>
+    </row>
+    <row r="63" spans="1:13" s="174" customFormat="1">
+      <c r="A63" s="28"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="33"/>
+      <c r="G63" s="175"/>
+      <c r="H63" s="176"/>
+      <c r="I63" s="177"/>
+      <c r="J63" s="177"/>
+      <c r="K63" s="177"/>
+      <c r="L63" s="171"/>
+      <c r="M63" s="12"/>
+    </row>
+    <row r="64" spans="1:13" s="174" customFormat="1">
+      <c r="A64" s="28"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="33"/>
+      <c r="G64" s="175"/>
+      <c r="H64" s="176"/>
+      <c r="I64" s="177"/>
+      <c r="J64" s="177"/>
+      <c r="K64" s="177"/>
+      <c r="L64" s="171"/>
+      <c r="M64" s="12"/>
+    </row>
+    <row r="65" spans="1:13" s="174" customFormat="1">
+      <c r="A65" s="28"/>
+      <c r="B65" s="171"/>
+      <c r="C65" s="171"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="33"/>
+      <c r="G65" s="175"/>
+      <c r="H65" s="176"/>
+      <c r="I65" s="177"/>
+      <c r="J65" s="177"/>
+      <c r="K65" s="177"/>
+      <c r="L65" s="171"/>
+      <c r="M65" s="12"/>
+    </row>
+    <row r="66" spans="1:13" s="174" customFormat="1">
+      <c r="A66" s="28"/>
+      <c r="B66" s="171"/>
+      <c r="C66" s="171"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="33"/>
+      <c r="G66" s="175"/>
+      <c r="H66" s="176"/>
+      <c r="I66" s="177"/>
+      <c r="J66" s="177"/>
+      <c r="K66" s="177"/>
+      <c r="L66" s="171"/>
+      <c r="M66" s="12"/>
+    </row>
+    <row r="67" spans="1:13" s="174" customFormat="1">
+      <c r="A67" s="28"/>
+      <c r="B67" s="171"/>
+      <c r="C67" s="171"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="33"/>
+      <c r="G67" s="175"/>
+      <c r="H67" s="176"/>
+      <c r="I67" s="177"/>
+      <c r="J67" s="177"/>
+      <c r="K67" s="177"/>
+      <c r="L67" s="171"/>
+      <c r="M67" s="12"/>
+    </row>
+    <row r="68" spans="1:13" s="174" customFormat="1">
+      <c r="A68" s="28"/>
+      <c r="B68" s="171"/>
+      <c r="C68" s="171"/>
+      <c r="D68" s="32"/>
+      <c r="E68" s="33"/>
+      <c r="G68" s="175"/>
+      <c r="H68" s="176"/>
+      <c r="I68" s="177"/>
+      <c r="J68" s="177"/>
+      <c r="K68" s="177"/>
+      <c r="L68" s="171"/>
+      <c r="M68" s="12"/>
+    </row>
+    <row r="69" spans="1:13" s="174" customFormat="1">
+      <c r="A69" s="28"/>
+      <c r="B69" s="171"/>
+      <c r="C69" s="171"/>
+      <c r="D69" s="172"/>
+      <c r="E69" s="173"/>
+      <c r="G69" s="175"/>
+      <c r="H69" s="176"/>
+      <c r="I69" s="177"/>
+      <c r="J69" s="177"/>
+      <c r="K69" s="177"/>
+      <c r="L69" s="171"/>
+      <c r="M69" s="12"/>
+    </row>
+    <row r="70" spans="1:13" s="174" customFormat="1">
+      <c r="A70" s="28"/>
+      <c r="B70" s="171"/>
+      <c r="C70" s="171"/>
+      <c r="D70" s="172"/>
+      <c r="E70" s="173"/>
+      <c r="G70" s="175"/>
+      <c r="H70" s="176"/>
+      <c r="I70" s="177"/>
+      <c r="J70" s="177"/>
+      <c r="K70" s="177"/>
+      <c r="L70" s="171"/>
+      <c r="M70" s="12"/>
+    </row>
+    <row r="71" spans="1:13" s="174" customFormat="1">
+      <c r="A71" s="28"/>
+      <c r="B71" s="171"/>
+      <c r="C71" s="171"/>
+      <c r="D71" s="172"/>
+      <c r="E71" s="173"/>
+      <c r="G71" s="175"/>
+      <c r="H71" s="176"/>
+      <c r="I71" s="177"/>
+      <c r="J71" s="177"/>
+      <c r="K71" s="177"/>
+      <c r="L71" s="171"/>
+      <c r="M71" s="12"/>
+    </row>
+    <row r="72" spans="1:13" s="174" customFormat="1">
+      <c r="A72" s="28"/>
+      <c r="B72" s="171"/>
+      <c r="C72" s="171"/>
+      <c r="D72" s="172"/>
+      <c r="E72" s="173"/>
+      <c r="G72" s="175"/>
+      <c r="H72" s="176"/>
+      <c r="I72" s="177"/>
+      <c r="J72" s="177"/>
+      <c r="K72" s="177"/>
+      <c r="L72" s="171"/>
+      <c r="M72" s="12"/>
+    </row>
+    <row r="73" spans="1:13" s="171" customFormat="1">
+      <c r="A73" s="28"/>
+      <c r="D73" s="172"/>
+      <c r="E73" s="173"/>
+      <c r="F73" s="174"/>
+      <c r="G73" s="175"/>
+      <c r="H73" s="176"/>
+      <c r="I73" s="177"/>
+      <c r="J73" s="177"/>
+      <c r="K73" s="177"/>
+      <c r="M73" s="12"/>
+    </row>
+    <row r="74" spans="1:13" s="171" customFormat="1">
+      <c r="A74" s="28"/>
+      <c r="D74" s="172"/>
+      <c r="E74" s="173"/>
+      <c r="F74" s="174"/>
+      <c r="G74" s="175"/>
+      <c r="H74" s="176"/>
+      <c r="I74" s="177"/>
+      <c r="J74" s="177"/>
+      <c r="K74" s="177"/>
+      <c r="M74" s="12"/>
+    </row>
+    <row r="75" spans="1:13" s="171" customFormat="1">
+      <c r="A75" s="28"/>
+      <c r="D75" s="172"/>
+      <c r="E75" s="173"/>
+      <c r="F75" s="174"/>
+      <c r="G75" s="175"/>
+      <c r="H75" s="176"/>
+      <c r="I75" s="177"/>
+      <c r="J75" s="177"/>
+      <c r="K75" s="177"/>
+      <c r="M75" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="K45:K46"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:H46"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:H7"/>
+    <mergeCell ref="A8:H8"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{182C79A2-D6C3-473F-AB84-010CAE2CDD23}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -7230,112 +8964,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="198" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="181"/>
-      <c r="F1" s="182"/>
-      <c r="G1" s="183"/>
-      <c r="H1" s="184"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="190"/>
+      <c r="E1" s="193"/>
+      <c r="F1" s="194"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="196"/>
     </row>
     <row r="2" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A2" s="213" t="s">
+      <c r="A2" s="223" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="214"/>
-      <c r="C2" s="214"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="216"/>
-      <c r="F2" s="215"/>
-      <c r="G2" s="217"/>
-      <c r="H2" s="218"/>
+      <c r="B2" s="218"/>
+      <c r="C2" s="218"/>
+      <c r="D2" s="224"/>
+      <c r="E2" s="225"/>
+      <c r="F2" s="224"/>
+      <c r="G2" s="226"/>
+      <c r="H2" s="227"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A3" s="219" t="s">
+      <c r="A3" s="228" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="214"/>
-      <c r="C3" s="214"/>
-      <c r="D3" s="215"/>
-      <c r="E3" s="216"/>
-      <c r="F3" s="215"/>
-      <c r="G3" s="217"/>
-      <c r="H3" s="218"/>
+      <c r="B3" s="218"/>
+      <c r="C3" s="218"/>
+      <c r="D3" s="224"/>
+      <c r="E3" s="225"/>
+      <c r="F3" s="224"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="227"/>
       <c r="I3" s="35"/>
       <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A4" s="210" t="s">
+      <c r="A4" s="220" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="212" t="s">
+      <c r="B4" s="222" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="211"/>
-      <c r="D4" s="211"/>
-      <c r="E4" s="211"/>
-      <c r="F4" s="211"/>
-      <c r="G4" s="211"/>
-      <c r="H4" s="211"/>
+      <c r="C4" s="221"/>
+      <c r="D4" s="221"/>
+      <c r="E4" s="221"/>
+      <c r="F4" s="221"/>
+      <c r="G4" s="221"/>
+      <c r="H4" s="221"/>
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A5" s="211"/>
-      <c r="B5" s="211"/>
-      <c r="C5" s="211"/>
-      <c r="D5" s="211"/>
-      <c r="E5" s="211"/>
-      <c r="F5" s="211"/>
-      <c r="G5" s="211"/>
-      <c r="H5" s="211"/>
+      <c r="A5" s="221"/>
+      <c r="B5" s="221"/>
+      <c r="C5" s="221"/>
+      <c r="D5" s="221"/>
+      <c r="E5" s="221"/>
+      <c r="F5" s="221"/>
+      <c r="G5" s="221"/>
+      <c r="H5" s="221"/>
       <c r="I5" s="35"/>
       <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="22.5" hidden="1" customHeight="1">
-      <c r="A6" s="210" t="s">
+      <c r="A6" s="220" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="212" t="s">
+      <c r="B6" s="222" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="211"/>
-      <c r="D6" s="211"/>
-      <c r="E6" s="211"/>
-      <c r="F6" s="211"/>
-      <c r="G6" s="211"/>
-      <c r="H6" s="211"/>
+      <c r="C6" s="221"/>
+      <c r="D6" s="221"/>
+      <c r="E6" s="221"/>
+      <c r="F6" s="221"/>
+      <c r="G6" s="221"/>
+      <c r="H6" s="221"/>
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
     </row>
     <row r="7" spans="1:12" ht="10.5" hidden="1" customHeight="1">
-      <c r="A7" s="211"/>
-      <c r="B7" s="211"/>
-      <c r="C7" s="211"/>
-      <c r="D7" s="211"/>
-      <c r="E7" s="211"/>
-      <c r="F7" s="211"/>
-      <c r="G7" s="211"/>
-      <c r="H7" s="211"/>
+      <c r="A7" s="221"/>
+      <c r="B7" s="221"/>
+      <c r="C7" s="221"/>
+      <c r="D7" s="221"/>
+      <c r="E7" s="221"/>
+      <c r="F7" s="221"/>
+      <c r="G7" s="221"/>
+      <c r="H7" s="221"/>
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A8" s="171" t="s">
+      <c r="A8" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="172"/>
-      <c r="C8" s="172"/>
-      <c r="D8" s="173"/>
-      <c r="E8" s="174"/>
-      <c r="F8" s="175"/>
-      <c r="G8" s="176"/>
-      <c r="H8" s="177"/>
+      <c r="B8" s="183"/>
+      <c r="C8" s="183"/>
+      <c r="D8" s="184"/>
+      <c r="E8" s="185"/>
+      <c r="F8" s="186"/>
+      <c r="G8" s="187"/>
+      <c r="H8" s="188"/>
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
     </row>
@@ -7700,16 +9434,16 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A20" s="206" t="s">
+      <c r="A20" s="182" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="172"/>
-      <c r="C20" s="172"/>
-      <c r="D20" s="173"/>
-      <c r="E20" s="174"/>
-      <c r="F20" s="175"/>
-      <c r="G20" s="176"/>
-      <c r="H20" s="177"/>
+      <c r="B20" s="183"/>
+      <c r="C20" s="183"/>
+      <c r="D20" s="184"/>
+      <c r="E20" s="185"/>
+      <c r="F20" s="186"/>
+      <c r="G20" s="187"/>
+      <c r="H20" s="188"/>
       <c r="I20" s="37">
         <v>0</v>
       </c>
@@ -7853,16 +9587,16 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A25" s="206" t="s">
+      <c r="A25" s="182" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="172"/>
-      <c r="C25" s="172"/>
-      <c r="D25" s="173"/>
-      <c r="E25" s="174"/>
-      <c r="F25" s="175"/>
-      <c r="G25" s="176"/>
-      <c r="H25" s="177"/>
+      <c r="B25" s="183"/>
+      <c r="C25" s="183"/>
+      <c r="D25" s="184"/>
+      <c r="E25" s="185"/>
+      <c r="F25" s="186"/>
+      <c r="G25" s="187"/>
+      <c r="H25" s="188"/>
       <c r="I25" s="37">
         <v>1</v>
       </c>
@@ -7946,16 +9680,16 @@
       <c r="L27" s="34"/>
     </row>
     <row r="28" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A28" s="206" t="s">
+      <c r="A28" s="182" t="s">
         <v>348</v>
       </c>
-      <c r="B28" s="172"/>
-      <c r="C28" s="172"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="174"/>
-      <c r="F28" s="175"/>
-      <c r="G28" s="176"/>
-      <c r="H28" s="177"/>
+      <c r="B28" s="183"/>
+      <c r="C28" s="183"/>
+      <c r="D28" s="184"/>
+      <c r="E28" s="185"/>
+      <c r="F28" s="186"/>
+      <c r="G28" s="187"/>
+      <c r="H28" s="188"/>
       <c r="I28" s="37"/>
       <c r="J28" s="36">
         <f>J27+I28</f>
@@ -8284,10 +10018,10 @@
       <c r="L37" s="12"/>
     </row>
     <row r="38" spans="1:12" ht="21" customHeight="1">
-      <c r="A38" s="207"/>
-      <c r="B38" s="179"/>
-      <c r="C38" s="179"/>
-      <c r="D38" s="180"/>
+      <c r="A38" s="189"/>
+      <c r="B38" s="181"/>
+      <c r="C38" s="181"/>
+      <c r="D38" s="190"/>
       <c r="E38" s="12"/>
       <c r="F38" s="43"/>
       <c r="G38" s="44"/>
@@ -8298,37 +10032,37 @@
       <c r="L38" s="12"/>
     </row>
     <row r="39" spans="1:12" ht="114" customHeight="1">
-      <c r="A39" s="220" t="s">
+      <c r="A39" s="217" t="s">
         <v>351</v>
       </c>
-      <c r="B39" s="214"/>
-      <c r="C39" s="214"/>
-      <c r="D39" s="209"/>
-      <c r="E39" s="181"/>
-      <c r="F39" s="182"/>
-      <c r="G39" s="183"/>
-      <c r="H39" s="184"/>
+      <c r="B39" s="218"/>
+      <c r="C39" s="218"/>
+      <c r="D39" s="192"/>
+      <c r="E39" s="193"/>
+      <c r="F39" s="194"/>
+      <c r="G39" s="195"/>
+      <c r="H39" s="196"/>
       <c r="I39" s="39"/>
       <c r="J39" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="K39" s="203"/>
+      <c r="K39" s="178"/>
       <c r="L39" s="12"/>
     </row>
     <row r="40" spans="1:12" ht="145.5" customHeight="1">
-      <c r="A40" s="221" t="s">
+      <c r="A40" s="219" t="s">
         <v>350</v>
       </c>
-      <c r="B40" s="214"/>
-      <c r="C40" s="214"/>
-      <c r="D40" s="180"/>
-      <c r="E40" s="181"/>
-      <c r="F40" s="182"/>
-      <c r="G40" s="183"/>
-      <c r="H40" s="184"/>
+      <c r="B40" s="218"/>
+      <c r="C40" s="218"/>
+      <c r="D40" s="190"/>
+      <c r="E40" s="193"/>
+      <c r="F40" s="194"/>
+      <c r="G40" s="195"/>
+      <c r="H40" s="196"/>
       <c r="I40" s="39"/>
       <c r="J40" s="52"/>
-      <c r="K40" s="204"/>
+      <c r="K40" s="179"/>
     </row>
     <row r="41" spans="1:12" ht="12.75" customHeight="1">
       <c r="A41" s="28"/>
@@ -8669,6 +10403,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:H7"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:H5"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="D39:H40"/>
     <mergeCell ref="K39:K40"/>
@@ -8678,13 +10419,6 @@
     <mergeCell ref="A25:H25"/>
     <mergeCell ref="A28:H28"/>
     <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:H7"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:H5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8692,14 +10426,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F42C2A-4DAD-47EC-9FF2-21B749D7E63A}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F9" sqref="F1:H1048576"/>
     </sheetView>
   </sheetViews>
@@ -8722,112 +10456,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="71.25" customHeight="1">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="198" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="181"/>
-      <c r="F1" s="182"/>
-      <c r="G1" s="183"/>
-      <c r="H1" s="184"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="190"/>
+      <c r="E1" s="193"/>
+      <c r="F1" s="194"/>
+      <c r="G1" s="195"/>
+      <c r="H1" s="196"/>
     </row>
     <row r="2" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A2" s="213" t="s">
+      <c r="A2" s="223" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="214"/>
-      <c r="C2" s="214"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="216"/>
-      <c r="F2" s="215"/>
-      <c r="G2" s="217"/>
-      <c r="H2" s="218"/>
+      <c r="B2" s="218"/>
+      <c r="C2" s="218"/>
+      <c r="D2" s="224"/>
+      <c r="E2" s="225"/>
+      <c r="F2" s="224"/>
+      <c r="G2" s="226"/>
+      <c r="H2" s="227"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A3" s="219" t="s">
+      <c r="A3" s="228" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="214"/>
-      <c r="C3" s="214"/>
-      <c r="D3" s="215"/>
-      <c r="E3" s="216"/>
-      <c r="F3" s="215"/>
-      <c r="G3" s="217"/>
-      <c r="H3" s="218"/>
+      <c r="B3" s="218"/>
+      <c r="C3" s="218"/>
+      <c r="D3" s="224"/>
+      <c r="E3" s="225"/>
+      <c r="F3" s="224"/>
+      <c r="G3" s="226"/>
+      <c r="H3" s="227"/>
       <c r="I3" s="35"/>
       <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A4" s="210" t="s">
+      <c r="A4" s="220" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="212" t="s">
+      <c r="B4" s="222" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="211"/>
-      <c r="D4" s="211"/>
-      <c r="E4" s="211"/>
-      <c r="F4" s="211"/>
-      <c r="G4" s="211"/>
-      <c r="H4" s="211"/>
+      <c r="C4" s="221"/>
+      <c r="D4" s="221"/>
+      <c r="E4" s="221"/>
+      <c r="F4" s="221"/>
+      <c r="G4" s="221"/>
+      <c r="H4" s="221"/>
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:12" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A5" s="211"/>
-      <c r="B5" s="211"/>
-      <c r="C5" s="211"/>
-      <c r="D5" s="211"/>
-      <c r="E5" s="211"/>
-      <c r="F5" s="211"/>
-      <c r="G5" s="211"/>
-      <c r="H5" s="211"/>
+      <c r="A5" s="221"/>
+      <c r="B5" s="221"/>
+      <c r="C5" s="221"/>
+      <c r="D5" s="221"/>
+      <c r="E5" s="221"/>
+      <c r="F5" s="221"/>
+      <c r="G5" s="221"/>
+      <c r="H5" s="221"/>
       <c r="I5" s="35"/>
       <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="22.5" hidden="1" customHeight="1">
-      <c r="A6" s="210" t="s">
+      <c r="A6" s="220" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="212" t="s">
+      <c r="B6" s="222" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="211"/>
-      <c r="D6" s="211"/>
-      <c r="E6" s="211"/>
-      <c r="F6" s="211"/>
-      <c r="G6" s="211"/>
-      <c r="H6" s="211"/>
+      <c r="C6" s="221"/>
+      <c r="D6" s="221"/>
+      <c r="E6" s="221"/>
+      <c r="F6" s="221"/>
+      <c r="G6" s="221"/>
+      <c r="H6" s="221"/>
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
     </row>
     <row r="7" spans="1:12" ht="10.5" hidden="1" customHeight="1">
-      <c r="A7" s="211"/>
-      <c r="B7" s="211"/>
-      <c r="C7" s="211"/>
-      <c r="D7" s="211"/>
-      <c r="E7" s="211"/>
-      <c r="F7" s="211"/>
-      <c r="G7" s="211"/>
-      <c r="H7" s="211"/>
+      <c r="A7" s="221"/>
+      <c r="B7" s="221"/>
+      <c r="C7" s="221"/>
+      <c r="D7" s="221"/>
+      <c r="E7" s="221"/>
+      <c r="F7" s="221"/>
+      <c r="G7" s="221"/>
+      <c r="H7" s="221"/>
       <c r="I7" s="35"/>
       <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A8" s="171" t="s">
+      <c r="A8" s="197" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="172"/>
-      <c r="C8" s="172"/>
-      <c r="D8" s="173"/>
-      <c r="E8" s="174"/>
-      <c r="F8" s="175"/>
-      <c r="G8" s="176"/>
-      <c r="H8" s="177"/>
+      <c r="B8" s="183"/>
+      <c r="C8" s="183"/>
+      <c r="D8" s="184"/>
+      <c r="E8" s="185"/>
+      <c r="F8" s="186"/>
+      <c r="G8" s="187"/>
+      <c r="H8" s="188"/>
       <c r="I8" s="35"/>
       <c r="J8" s="35"/>
     </row>
@@ -9192,16 +10926,16 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A20" s="206" t="s">
+      <c r="A20" s="182" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="172"/>
-      <c r="C20" s="172"/>
-      <c r="D20" s="173"/>
-      <c r="E20" s="174"/>
-      <c r="F20" s="175"/>
-      <c r="G20" s="176"/>
-      <c r="H20" s="177"/>
+      <c r="B20" s="183"/>
+      <c r="C20" s="183"/>
+      <c r="D20" s="184"/>
+      <c r="E20" s="185"/>
+      <c r="F20" s="186"/>
+      <c r="G20" s="187"/>
+      <c r="H20" s="188"/>
       <c r="I20" s="37">
         <v>0</v>
       </c>
@@ -9345,16 +11079,16 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A25" s="206" t="s">
+      <c r="A25" s="182" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="172"/>
-      <c r="C25" s="172"/>
-      <c r="D25" s="173"/>
-      <c r="E25" s="174"/>
-      <c r="F25" s="175"/>
-      <c r="G25" s="176"/>
-      <c r="H25" s="177"/>
+      <c r="B25" s="183"/>
+      <c r="C25" s="183"/>
+      <c r="D25" s="184"/>
+      <c r="E25" s="185"/>
+      <c r="F25" s="186"/>
+      <c r="G25" s="187"/>
+      <c r="H25" s="188"/>
       <c r="I25" s="37">
         <v>1</v>
       </c>
@@ -9510,16 +11244,16 @@
       <c r="L29" s="34"/>
     </row>
     <row r="30" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A30" s="206" t="s">
+      <c r="A30" s="182" t="s">
         <v>348</v>
       </c>
-      <c r="B30" s="172"/>
-      <c r="C30" s="172"/>
-      <c r="D30" s="173"/>
-      <c r="E30" s="174"/>
-      <c r="F30" s="175"/>
-      <c r="G30" s="176"/>
-      <c r="H30" s="177"/>
+      <c r="B30" s="183"/>
+      <c r="C30" s="183"/>
+      <c r="D30" s="184"/>
+      <c r="E30" s="185"/>
+      <c r="F30" s="186"/>
+      <c r="G30" s="187"/>
+      <c r="H30" s="188"/>
       <c r="I30" s="37"/>
       <c r="J30" s="36">
         <f>J29+I30</f>
@@ -9885,10 +11619,10 @@
       <c r="L40" s="12"/>
     </row>
     <row r="41" spans="1:12" ht="21" customHeight="1">
-      <c r="A41" s="207"/>
-      <c r="B41" s="179"/>
-      <c r="C41" s="179"/>
-      <c r="D41" s="180"/>
+      <c r="A41" s="189"/>
+      <c r="B41" s="181"/>
+      <c r="C41" s="181"/>
+      <c r="D41" s="190"/>
       <c r="E41" s="12"/>
       <c r="F41" s="43"/>
       <c r="G41" s="44"/>
@@ -9899,37 +11633,37 @@
       <c r="L41" s="12"/>
     </row>
     <row r="42" spans="1:12" ht="114" customHeight="1">
-      <c r="A42" s="220" t="s">
+      <c r="A42" s="217" t="s">
         <v>351</v>
       </c>
-      <c r="B42" s="214"/>
-      <c r="C42" s="214"/>
-      <c r="D42" s="209"/>
-      <c r="E42" s="181"/>
-      <c r="F42" s="182"/>
-      <c r="G42" s="183"/>
-      <c r="H42" s="184"/>
+      <c r="B42" s="218"/>
+      <c r="C42" s="218"/>
+      <c r="D42" s="192"/>
+      <c r="E42" s="193"/>
+      <c r="F42" s="194"/>
+      <c r="G42" s="195"/>
+      <c r="H42" s="196"/>
       <c r="I42" s="39"/>
       <c r="J42" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="K42" s="203"/>
+      <c r="K42" s="178"/>
       <c r="L42" s="12"/>
     </row>
     <row r="43" spans="1:12" ht="145.5" customHeight="1">
-      <c r="A43" s="221" t="s">
+      <c r="A43" s="219" t="s">
         <v>350</v>
       </c>
-      <c r="B43" s="214"/>
-      <c r="C43" s="214"/>
-      <c r="D43" s="180"/>
-      <c r="E43" s="181"/>
-      <c r="F43" s="182"/>
-      <c r="G43" s="183"/>
-      <c r="H43" s="184"/>
+      <c r="B43" s="218"/>
+      <c r="C43" s="218"/>
+      <c r="D43" s="190"/>
+      <c r="E43" s="193"/>
+      <c r="F43" s="194"/>
+      <c r="G43" s="195"/>
+      <c r="H43" s="196"/>
       <c r="I43" s="39"/>
       <c r="J43" s="52"/>
-      <c r="K43" s="204"/>
+      <c r="K43" s="179"/>
     </row>
     <row r="44" spans="1:12" ht="12.75" customHeight="1">
       <c r="A44" s="28"/>
@@ -10270,6 +12004,10 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A8:H8"/>
     <mergeCell ref="K42:K43"/>
     <mergeCell ref="A43:C43"/>
     <mergeCell ref="B4:H5"/>
@@ -10282,10 +12020,6 @@
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="D42:H43"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A8:H8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10293,11 +12027,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:CC68"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="S69" sqref="S67:S69"/>
     </sheetView>
   </sheetViews>

</xml_diff>